<commit_message>
parameters: markers and effect direction
1. when swiping - a circle will apear above parameters that are going to be affected. small circle for small effect and large circle  for large.
2. When parameter changes it is painted in red or green according to the direction of change down or up. for a little while
3. SwipeManager.EndGameDueParam() - empty methos that should handle the case that some parameter reached its limit (0 or 1) - to be continued
</commit_message>
<xml_diff>
--- a/Assets/Excel/bibiCards.xlsx
+++ b/Assets/Excel/bibiCards.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinalevy-new/Dropbox/part 3/courses 3/unity files/bibiking/Assets/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinalevy-new/Dropbox/part 3/courses 3/unity files/Git/BibikingCards/Assets/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="98">
   <si>
     <t>בטחון</t>
   </si>
@@ -132,24 +132,9 @@
     <t>credit</t>
   </si>
   <si>
-    <t>קואליציה</t>
-  </si>
-  <si>
-    <t>שרים</t>
-  </si>
-  <si>
-    <t>אופוזיציה</t>
-  </si>
-  <si>
     <t>טראמפ</t>
   </si>
   <si>
-    <t>האבטלה ירדה, אבל הגירעון עולה והכלכלה מתערערת</t>
-  </si>
-  <si>
-    <t>לקצץ בחינוך. מי ישים לב?</t>
-  </si>
-  <si>
     <t>איילת שקד</t>
   </si>
   <si>
@@ -162,9 +147,6 @@
     <t>מפכ"ל המשטרה</t>
   </si>
   <si>
-    <t>נפתחה נגדך חקירה על שחיתות, אני צריך שתגיע לחקירה</t>
-  </si>
-  <si>
     <t>אני לא מקבל הוראות מהדיפ סטייט</t>
   </si>
   <si>
@@ -180,45 +162,12 @@
     <t>זאב ז'בוטינסקי</t>
   </si>
   <si>
-    <t>אותרה דליפה בכור, אך נראה כי הצלחנו להשתלט עליה</t>
-  </si>
-  <si>
-    <t>טראמפ הוריד ממך עוקב באינסטה</t>
-  </si>
-  <si>
-    <t>שטויות, למי אכפת</t>
-  </si>
-  <si>
-    <t>אני צריך לנסוע מיד לארה״ב, זוהי שעת חירום</t>
-  </si>
-  <si>
     <t>מירי רגב</t>
   </si>
   <si>
-    <t>ישראל כ״ץ</t>
-  </si>
-  <si>
-    <t>להטיל מיסים על עסקים קטנים</t>
-  </si>
-  <si>
     <t>בנט מחרפן אותי, אני רוצה מקום בליכוד. נוכל להיפגש בארבע עיניים?</t>
   </si>
   <si>
-    <t>אני נותן לך את תיק הביטחון </t>
-  </si>
-  <si>
-    <t>תקים קזינו בירושלים תמורת ארבעה מטוסים </t>
-  </si>
-  <si>
-    <t>חמישה מטוסים וסגרנו</t>
-  </si>
-  <si>
-    <t>אני מוכן להקים בית כנסת בכיכר רבין על שמך</t>
-  </si>
-  <si>
-    <t>תקצץ 20% מהמשכורת של העוזרת. מצאתי פירור של עוגייה על הרצפה</t>
-  </si>
-  <si>
     <t>דבר עם מימון</t>
   </si>
   <si>
@@ -228,30 +177,15 @@
     <t>בפגישה הבאה עם טראמפ אני מבקשת שלא תצטרף </t>
   </si>
   <si>
-    <t>אין בעיה רעייתי, אני אעביר את הזמן עם מלאניה</t>
-  </si>
-  <si>
-    <t>תדאג שיוקם בניין על שמי בפקולטה לפסיכולוגיה </t>
-  </si>
-  <si>
     <t>אבא, תקנה לי ערוץ טלוויזיה משלי</t>
   </si>
   <si>
     <t>אני מעביר לך את התאגיד</t>
   </si>
   <si>
-    <t>נתחיל מתכנית בערוץ 20</t>
-  </si>
-  <si>
     <t>שוב קמתי בחושך ולבשתי את המכנסיים הפוך. אני דורש לבטל את שעון הקיץ לנצח</t>
   </si>
   <si>
-    <t>הכביסה של שרה לא תספיק להתייבש</t>
-  </si>
-  <si>
-    <t>לך על זה</t>
-  </si>
-  <si>
     <t>ארגוני הנשים חסמו את הדרך למעון בבלפור </t>
   </si>
   <si>
@@ -285,73 +219,109 @@
     <t>אבא, פתחתי לך טיק טוק. תבחר שיר</t>
   </si>
   <si>
-    <t>"לא קלה היא דרכנו" </t>
-  </si>
-  <si>
     <t>תשאיר ככה, אני נואם באו"ם בשבוע הבא</t>
   </si>
   <si>
     <t>תחזיר לסגול חציל</t>
   </si>
   <si>
-    <t>תשלח לו 500 עותקים של דף המסרים</t>
-  </si>
-  <si>
-    <t>הוא כבר לא רלוונטי. תשלח לו זימון לשימוע</t>
-  </si>
-  <si>
     <t>(נגלה אליך בחלום): ״בנימין, זוהי לא דרכי. אין מקום להסתה ולפילוג בקרב אזרחי ישראל״</t>
   </si>
   <si>
     <t>סבבה, אני מבטל את חוק הלאום</t>
   </si>
   <si>
-    <t>נתת לי רעיון, מחר מצודת זאב תיעלם </t>
-  </si>
-  <si>
     <t>אמיר אוחנה</t>
   </si>
   <si>
     <t>הזדמנות להפשיר קרקעות לקבלנים</t>
   </si>
   <si>
-    <t>עוזרת סדרנית במרכז הליכוד</t>
-  </si>
-  <si>
-    <t>אבא, אתה יכול לפרגן לי 400 שקל?</t>
+    <t>בני גנץ</t>
+  </si>
+  <si>
+    <t>הרמטכ״ל</t>
+  </si>
+  <si>
+    <t>בלוני התבערה הפכו לרחפנים ממולכדים. חייבים לחסל את החמאס</t>
+  </si>
+  <si>
+    <t>בוא נחכה, אולי אחרי האירוויזיון</t>
+  </si>
+  <si>
+    <t>באת לי בול בזמן</t>
+  </si>
+  <si>
+    <t>אוקיי, אפשר לדבר על תיק הביטחון</t>
+  </si>
+  <si>
+    <t>אוקיי, תרצי להיות מפיקת הליכודיאדה? </t>
+  </si>
+  <si>
+    <t>מייק איזראל גרייט אגיין ותקים על שמי קזינו בירושלים. אני אתן לך ארבע צוללות </t>
+  </si>
+  <si>
+    <t>חמש צוללות וסגרנו</t>
+  </si>
+  <si>
+    <t>אני מוכן לקרוא לכיכר רבין על שמך </t>
+  </si>
+  <si>
+    <t>תקצץ חצי ממשכורת העוזרת, מצאתי גרביים במקרר</t>
+  </si>
+  <si>
+    <t>אבא, אתה יכול לפרגן לי ארבע מאות שקל?</t>
+  </si>
+  <si>
+    <t>תדאג שיוקם בניין על שמי בפקולטה לפסיכולוגיה באוניברסיטת תל אביב</t>
+  </si>
+  <si>
+    <t>נתחיל מתכנית בערוץ עשרים</t>
+  </si>
+  <si>
+    <t>סורי, הכביסה של שרה לא תספיק להתייבש</t>
+  </si>
+  <si>
+    <t>אין בעיה, לך על זה </t>
+  </si>
+  <si>
+    <t>נפתחה נגדך חקירה על שחיתות, אני צריך שתגיע לכאן</t>
+  </si>
+  <si>
+    <t>"אתה תותח"</t>
+  </si>
+  <si>
+    <t>"I Will Survive"</t>
+  </si>
+  <si>
+    <t>יניב מלכה, מעצב שיער</t>
+  </si>
+  <si>
+    <t>תשלח לו חמש מאות עותקים של דף המסרים</t>
+  </si>
+  <si>
+    <t>תשלח לו זימון לשימוע</t>
+  </si>
+  <si>
+    <t>אתה מפריע לי לישון</t>
+  </si>
+  <si>
+    <t>אותרה דליפה בכור בדימונה, אך נראה כי הצלחנו להשתלט עליה</t>
+  </si>
+  <si>
+    <t>לבי עם תושבי דימונה</t>
+  </si>
+  <si>
+    <t>עברו שנתיים, עכשיו תורי</t>
+  </si>
+  <si>
+    <t>כמובן, הבטחתי לקיים וכך אעשה</t>
+  </si>
+  <si>
+    <t>חחחחחחחחחחחחחח</t>
   </si>
   <si>
     <t>אריה דרעי</t>
-  </si>
-  <si>
-    <t>״אני אשרוד״</t>
-  </si>
-  <si>
-    <t>צריך להסתיר ולטייח שלא יירדו המחירים</t>
-  </si>
-  <si>
-    <t>יאיר נתניהו </t>
-  </si>
-  <si>
-    <t>בני גנץ</t>
-  </si>
-  <si>
-    <t>עברו שנתיים, תורי להיות ראש הממשלה</t>
-  </si>
-  <si>
-    <t>כמובן, הבטחתי לקיים את הרוטציה וכך אעשה</t>
-  </si>
-  <si>
-    <t>חחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחח</t>
-  </si>
-  <si>
-    <t>בוא לטעום את עוגת השכבות שהכנתי לקראת האודישן למאסטר שף</t>
-  </si>
-  <si>
-    <t>לטעום ולהקיא</t>
-  </si>
-  <si>
-    <t>לטעום ולקבל קלקול קיבה</t>
   </si>
 </sst>
 </file>
@@ -454,7 +424,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -472,9 +442,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -754,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -822,47 +789,44 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
-        <v>50</v>
+      <c r="A2" s="9">
+        <v>31</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="8">
-        <v>5</v>
-      </c>
-      <c r="G2" s="8">
-        <v>2</v>
-      </c>
-      <c r="H2" s="8">
-        <v>5</v>
-      </c>
-      <c r="I2" s="8">
-        <v>4</v>
-      </c>
-      <c r="J2" s="8">
-        <v>5</v>
-      </c>
-      <c r="K2" s="8">
-        <v>3</v>
-      </c>
-      <c r="L2" s="8">
-        <v>3</v>
-      </c>
-      <c r="M2" s="8">
-        <v>3</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>35</v>
+        <v>70</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0</v>
+      </c>
+      <c r="G2" s="7">
+        <v>5</v>
+      </c>
+      <c r="H2" s="7">
+        <v>2</v>
+      </c>
+      <c r="I2" s="7">
+        <v>5</v>
+      </c>
+      <c r="J2" s="7">
+        <v>8</v>
+      </c>
+      <c r="K2" s="10">
+        <v>2</v>
+      </c>
+      <c r="L2" s="7">
+        <v>10</v>
+      </c>
+      <c r="M2" s="7">
+        <v>5</v>
       </c>
       <c r="O2" s="8">
         <v>3</v>
@@ -873,43 +837,40 @@
         <v>51</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="F3" s="8">
-        <v>2</v>
-      </c>
-      <c r="G3" s="8">
-        <v>4</v>
-      </c>
-      <c r="H3" s="8">
-        <v>1</v>
-      </c>
-      <c r="I3" s="8">
-        <v>3</v>
-      </c>
-      <c r="J3" s="8">
-        <v>2</v>
-      </c>
-      <c r="K3" s="8">
-        <v>1</v>
-      </c>
-      <c r="L3" s="8">
-        <v>4</v>
-      </c>
-      <c r="M3" s="8">
+        <v>75</v>
+      </c>
+      <c r="F3">
         <v>0</v>
       </c>
-      <c r="N3" t="s">
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
         <v>0</v>
+      </c>
+      <c r="J3">
+        <v>5</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>10</v>
       </c>
       <c r="O3" s="8">
         <v>3</v>
@@ -920,42 +881,39 @@
         <v>52</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" s="8">
-        <v>1</v>
-      </c>
-      <c r="G4" s="8">
-        <v>1</v>
-      </c>
-      <c r="H4" s="8">
-        <v>1</v>
-      </c>
-      <c r="I4" s="8">
-        <v>1</v>
-      </c>
-      <c r="J4" s="8">
-        <v>4</v>
-      </c>
-      <c r="K4" s="8">
-        <v>3</v>
-      </c>
-      <c r="L4" s="8">
-        <v>2</v>
-      </c>
-      <c r="M4" s="8">
-        <v>3</v>
-      </c>
-      <c r="N4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>10</v>
+      </c>
+      <c r="M4">
         <v>5</v>
       </c>
       <c r="O4" s="8">
@@ -970,7 +928,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>6</v>
@@ -978,32 +936,29 @@
       <c r="E5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="10">
-        <v>1</v>
-      </c>
-      <c r="G5" s="10">
-        <v>2</v>
-      </c>
-      <c r="H5" s="10">
-        <v>3</v>
-      </c>
-      <c r="I5" s="10">
-        <v>4</v>
-      </c>
-      <c r="J5" s="10">
-        <v>1</v>
-      </c>
-      <c r="K5" s="10">
-        <v>2</v>
-      </c>
-      <c r="L5" s="10">
-        <v>3</v>
-      </c>
-      <c r="M5" s="10">
-        <v>4</v>
-      </c>
-      <c r="N5" t="s">
-        <v>9</v>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <v>8</v>
       </c>
       <c r="O5" s="10">
         <v>3</v>
@@ -1014,42 +969,39 @@
         <v>54</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="10">
-        <v>1</v>
-      </c>
-      <c r="G6" s="10">
-        <v>2</v>
-      </c>
-      <c r="H6" s="10">
-        <v>3</v>
-      </c>
-      <c r="I6" s="10">
-        <v>4</v>
-      </c>
-      <c r="J6" s="10">
-        <v>1</v>
-      </c>
-      <c r="K6" s="10">
-        <v>2</v>
-      </c>
-      <c r="L6" s="10">
-        <v>3</v>
-      </c>
-      <c r="M6" s="10">
-        <v>4</v>
-      </c>
-      <c r="N6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>8</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <v>5</v>
+      </c>
+      <c r="M6">
         <v>0</v>
       </c>
       <c r="O6" s="10">
@@ -1061,43 +1013,40 @@
         <v>55</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" s="10">
-        <v>1</v>
-      </c>
-      <c r="G7" s="10">
-        <v>2</v>
-      </c>
-      <c r="H7" s="10">
-        <v>3</v>
-      </c>
-      <c r="I7" s="10">
-        <v>4</v>
-      </c>
-      <c r="J7" s="10">
-        <v>1</v>
-      </c>
-      <c r="K7" s="10">
-        <v>2</v>
-      </c>
-      <c r="L7" s="10">
-        <v>3</v>
-      </c>
-      <c r="M7" s="10">
-        <v>4</v>
-      </c>
-      <c r="N7" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>8</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7">
+        <v>5</v>
+      </c>
+      <c r="M7">
+        <v>8</v>
       </c>
       <c r="O7" s="10">
         <v>3</v>
@@ -1108,10 +1057,10 @@
         <v>56</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>6</v>
@@ -1119,32 +1068,29 @@
       <c r="E8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="10">
-        <v>1</v>
-      </c>
-      <c r="G8" s="10">
-        <v>2</v>
-      </c>
-      <c r="H8" s="10">
-        <v>3</v>
-      </c>
-      <c r="I8" s="10">
-        <v>4</v>
-      </c>
-      <c r="J8" s="10">
-        <v>1</v>
-      </c>
-      <c r="K8" s="10">
-        <v>2</v>
-      </c>
-      <c r="L8" s="10">
-        <v>3</v>
-      </c>
-      <c r="M8" s="10">
-        <v>4</v>
-      </c>
-      <c r="N8" t="s">
-        <v>9</v>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>8</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
+      </c>
+      <c r="M8">
+        <v>8</v>
       </c>
       <c r="O8" s="10">
         <v>3</v>
@@ -1155,43 +1101,40 @@
         <v>57</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="10">
-        <v>1</v>
-      </c>
-      <c r="G9" s="10">
-        <v>2</v>
-      </c>
-      <c r="H9" s="10">
-        <v>3</v>
-      </c>
-      <c r="I9" s="10">
-        <v>4</v>
-      </c>
-      <c r="J9" s="10">
-        <v>1</v>
-      </c>
-      <c r="K9" s="10">
-        <v>2</v>
-      </c>
-      <c r="L9" s="10">
-        <v>3</v>
-      </c>
-      <c r="M9" s="10">
-        <v>4</v>
-      </c>
-      <c r="N9" t="s">
-        <v>5</v>
+        <v>82</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>10</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>5</v>
+      </c>
+      <c r="L9">
+        <v>10</v>
+      </c>
+      <c r="M9">
+        <v>8</v>
       </c>
       <c r="O9" s="10">
         <v>3</v>
@@ -1205,40 +1148,37 @@
         <v>97</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F10" s="8">
-        <v>5</v>
-      </c>
-      <c r="G10" s="10">
-        <v>2</v>
-      </c>
-      <c r="H10" s="10">
-        <v>3</v>
-      </c>
-      <c r="I10" s="10">
-        <v>4</v>
-      </c>
-      <c r="J10" s="10">
-        <v>1</v>
-      </c>
-      <c r="K10" s="10">
-        <v>2</v>
-      </c>
-      <c r="L10" s="10">
-        <v>3</v>
-      </c>
-      <c r="M10" s="10">
-        <v>4</v>
-      </c>
-      <c r="N10" t="s">
-        <v>34</v>
+        <v>84</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>8</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>5</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
       </c>
       <c r="O10" s="10">
         <v>3</v>
@@ -1252,40 +1192,37 @@
         <v>13</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11" s="8">
-        <v>1</v>
-      </c>
-      <c r="G11" s="10">
-        <v>2</v>
-      </c>
-      <c r="H11" s="10">
-        <v>3</v>
-      </c>
-      <c r="I11" s="10">
-        <v>4</v>
-      </c>
-      <c r="J11" s="10">
-        <v>1</v>
-      </c>
-      <c r="K11" s="10">
-        <v>2</v>
-      </c>
-      <c r="L11" s="10">
-        <v>3</v>
-      </c>
-      <c r="M11" s="10">
-        <v>4</v>
-      </c>
-      <c r="N11" t="s">
-        <v>35</v>
+        <v>54</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>8</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="J11">
+        <v>5</v>
+      </c>
+      <c r="K11">
+        <v>5</v>
+      </c>
+      <c r="L11">
+        <v>5</v>
+      </c>
+      <c r="M11">
+        <v>2</v>
       </c>
       <c r="O11" s="10">
         <v>3</v>
@@ -1296,43 +1233,40 @@
         <v>61</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="10">
-        <v>1</v>
-      </c>
-      <c r="G12" s="10">
-        <v>2</v>
-      </c>
-      <c r="H12" s="10">
-        <v>3</v>
-      </c>
-      <c r="I12" s="10">
-        <v>4</v>
-      </c>
-      <c r="J12" s="10">
-        <v>1</v>
-      </c>
-      <c r="K12" s="10">
-        <v>2</v>
-      </c>
-      <c r="L12" s="10">
-        <v>3</v>
-      </c>
-      <c r="M12" s="10">
-        <v>4</v>
-      </c>
-      <c r="N12" t="s">
-        <v>35</v>
+        <v>39</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+      <c r="I12">
+        <v>5</v>
+      </c>
+      <c r="J12">
+        <v>5</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>10</v>
+      </c>
+      <c r="M12">
+        <v>5</v>
       </c>
       <c r="O12" s="10">
         <v>3</v>
@@ -1343,43 +1277,40 @@
         <v>62</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F13" s="10">
-        <v>1</v>
-      </c>
-      <c r="G13" s="8">
-        <v>2</v>
-      </c>
-      <c r="H13" s="8">
-        <v>5</v>
-      </c>
-      <c r="I13" s="8">
-        <v>4</v>
-      </c>
-      <c r="J13" s="8">
-        <v>5</v>
-      </c>
-      <c r="K13" s="8">
-        <v>3</v>
-      </c>
-      <c r="L13" s="8">
-        <v>3</v>
-      </c>
-      <c r="M13" s="8">
-        <v>3</v>
-      </c>
-      <c r="N13" t="s">
-        <v>36</v>
+        <v>58</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+      <c r="H13">
+        <v>5</v>
+      </c>
+      <c r="I13">
+        <v>8</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>5</v>
+      </c>
+      <c r="L13">
+        <v>5</v>
+      </c>
+      <c r="M13">
+        <v>8</v>
       </c>
       <c r="O13" s="8">
         <v>3</v>
@@ -1390,43 +1321,40 @@
         <v>63</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F14" s="10">
-        <v>1</v>
-      </c>
-      <c r="G14" s="8">
-        <v>4</v>
-      </c>
-      <c r="H14" s="8">
-        <v>1</v>
-      </c>
-      <c r="I14" s="8">
-        <v>3</v>
-      </c>
-      <c r="J14" s="8">
-        <v>2</v>
-      </c>
-      <c r="K14" s="8">
-        <v>1</v>
-      </c>
-      <c r="L14" s="8">
-        <v>4</v>
-      </c>
-      <c r="M14" s="8">
+        <v>61</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14" s="4">
         <v>0</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>35</v>
+      <c r="I14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <v>5</v>
+      </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
+      <c r="L14">
+        <v>10</v>
+      </c>
+      <c r="M14">
+        <v>5</v>
       </c>
       <c r="O14" s="8">
         <v>3</v>
@@ -1437,43 +1365,40 @@
         <v>64</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>85</v>
+        <v>62</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="F15" s="10">
-        <v>1</v>
-      </c>
-      <c r="G15" s="8">
-        <v>1</v>
-      </c>
-      <c r="H15" s="8">
-        <v>1</v>
-      </c>
-      <c r="I15" s="8">
-        <v>1</v>
-      </c>
-      <c r="J15" s="8">
-        <v>4</v>
-      </c>
-      <c r="K15" s="8">
-        <v>3</v>
-      </c>
-      <c r="L15" s="8">
-        <v>2</v>
-      </c>
-      <c r="M15" s="8">
-        <v>3</v>
-      </c>
-      <c r="N15" t="s">
-        <v>0</v>
+        <v>87</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <v>5</v>
+      </c>
+      <c r="I15">
+        <v>8</v>
+      </c>
+      <c r="J15">
+        <v>5</v>
+      </c>
+      <c r="K15">
+        <v>5</v>
+      </c>
+      <c r="L15">
+        <v>5</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
       </c>
       <c r="O15" s="8">
         <v>3</v>
@@ -1484,43 +1409,40 @@
         <v>65</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F16" s="10">
-        <v>1</v>
-      </c>
-      <c r="G16" s="10">
-        <v>2</v>
-      </c>
-      <c r="H16" s="10">
-        <v>3</v>
-      </c>
-      <c r="I16" s="10">
-        <v>4</v>
-      </c>
-      <c r="J16" s="10">
-        <v>1</v>
-      </c>
-      <c r="K16" s="10">
-        <v>2</v>
-      </c>
-      <c r="L16" s="10">
-        <v>3</v>
-      </c>
-      <c r="M16" s="10">
-        <v>4</v>
-      </c>
-      <c r="N16" t="s">
-        <v>5</v>
+        <v>64</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <v>5</v>
+      </c>
+      <c r="K16">
+        <v>5</v>
+      </c>
+      <c r="L16">
+        <v>5</v>
+      </c>
+      <c r="M16">
+        <v>8</v>
       </c>
       <c r="O16" s="10">
         <v>3</v>
@@ -1534,40 +1456,37 @@
         <v>13</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="F17" s="10">
-        <v>1</v>
-      </c>
-      <c r="G17" s="10">
-        <v>2</v>
-      </c>
-      <c r="H17" s="10">
-        <v>3</v>
-      </c>
-      <c r="I17" s="10">
-        <v>4</v>
-      </c>
-      <c r="J17" s="10">
-        <v>1</v>
-      </c>
-      <c r="K17" s="10">
-        <v>2</v>
-      </c>
-      <c r="L17" s="10">
-        <v>3</v>
-      </c>
-      <c r="M17" s="10">
-        <v>4</v>
-      </c>
-      <c r="N17" t="s">
-        <v>9</v>
+        <v>90</v>
+      </c>
+      <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="J17">
+        <v>5</v>
+      </c>
+      <c r="K17">
+        <v>5</v>
+      </c>
+      <c r="L17">
+        <v>5</v>
+      </c>
+      <c r="M17">
+        <v>5</v>
       </c>
       <c r="O17" s="10">
         <v>3</v>
@@ -1578,43 +1497,40 @@
         <v>67</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="D18" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="F18" s="10">
-        <v>1</v>
-      </c>
-      <c r="G18" s="10">
-        <v>2</v>
-      </c>
-      <c r="H18" s="10">
-        <v>3</v>
-      </c>
-      <c r="I18" s="10">
-        <v>4</v>
-      </c>
-      <c r="J18" s="10">
-        <v>1</v>
-      </c>
-      <c r="K18" s="10">
-        <v>2</v>
-      </c>
-      <c r="L18" s="10">
-        <v>3</v>
-      </c>
-      <c r="M18" s="10">
-        <v>4</v>
-      </c>
-      <c r="N18" t="s">
+      <c r="F18">
+        <v>10</v>
+      </c>
+      <c r="G18">
+        <v>8</v>
+      </c>
+      <c r="H18">
         <v>0</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <v>5</v>
+      </c>
+      <c r="K18">
+        <v>5</v>
+      </c>
+      <c r="L18">
+        <v>5</v>
+      </c>
+      <c r="M18">
+        <v>5</v>
       </c>
       <c r="O18" s="10">
         <v>3</v>
@@ -1625,195 +1541,119 @@
         <v>68</v>
       </c>
       <c r="B19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="9" t="s">
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>5</v>
+      </c>
+      <c r="I19">
+        <v>8</v>
+      </c>
+      <c r="J19">
+        <v>5</v>
+      </c>
+      <c r="K19">
+        <v>5</v>
+      </c>
+      <c r="L19">
+        <v>5</v>
+      </c>
+      <c r="M19">
+        <v>5</v>
+      </c>
+      <c r="O19" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>71</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F19" s="10">
-        <v>1</v>
-      </c>
-      <c r="G19" s="10">
-        <v>2</v>
-      </c>
-      <c r="H19" s="10">
-        <v>3</v>
-      </c>
-      <c r="I19" s="10">
-        <v>4</v>
-      </c>
-      <c r="J19" s="10">
-        <v>1</v>
-      </c>
-      <c r="K19" s="10">
-        <v>2</v>
-      </c>
-      <c r="L19" s="10">
-        <v>3</v>
-      </c>
-      <c r="M19" s="10">
-        <v>4</v>
-      </c>
-      <c r="N19" t="s">
-        <v>5</v>
-      </c>
-      <c r="O19" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="7">
-        <v>70</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>51</v>
-      </c>
       <c r="D20" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="8">
-        <v>5</v>
-      </c>
-      <c r="G20" s="10">
-        <v>2</v>
-      </c>
-      <c r="H20" s="10">
-        <v>3</v>
-      </c>
-      <c r="I20" s="10">
-        <v>4</v>
-      </c>
-      <c r="J20" s="10">
-        <v>1</v>
-      </c>
-      <c r="K20" s="10">
-        <v>2</v>
-      </c>
-      <c r="L20" s="10">
-        <v>3</v>
-      </c>
-      <c r="M20" s="10">
-        <v>4</v>
-      </c>
-      <c r="N20" t="s">
-        <v>5</v>
-      </c>
-      <c r="O20" s="10">
+        <v>95</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F20" s="9">
+        <v>5</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>5</v>
+      </c>
+      <c r="I20">
+        <v>5</v>
+      </c>
+      <c r="J20">
+        <v>5</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>5</v>
+      </c>
+      <c r="M20">
+        <v>5</v>
+      </c>
+      <c r="O20" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>71</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="F21" s="8">
-        <v>5</v>
-      </c>
-      <c r="G21" s="10">
-        <v>2</v>
-      </c>
-      <c r="H21" s="10">
-        <v>3</v>
-      </c>
-      <c r="I21" s="10">
-        <v>4</v>
-      </c>
-      <c r="J21" s="10">
-        <v>1</v>
-      </c>
-      <c r="K21" s="10">
-        <v>2</v>
-      </c>
-      <c r="L21" s="10">
-        <v>3</v>
-      </c>
-      <c r="M21" s="10">
-        <v>4</v>
-      </c>
-      <c r="N21" t="s">
-        <v>5</v>
-      </c>
-      <c r="O21" s="7">
-        <v>10</v>
-      </c>
+      <c r="A21" s="4"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="4"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="7">
-        <v>74</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="F22" s="8">
-        <v>5</v>
-      </c>
-      <c r="G22" s="10">
-        <v>2</v>
-      </c>
-      <c r="H22" s="10">
-        <v>3</v>
-      </c>
-      <c r="I22" s="10">
-        <v>4</v>
-      </c>
-      <c r="J22" s="10">
-        <v>1</v>
-      </c>
-      <c r="K22" s="10">
-        <v>2</v>
-      </c>
-      <c r="L22" s="10">
-        <v>3</v>
-      </c>
-      <c r="M22" s="10">
-        <v>4</v>
-      </c>
-      <c r="N22" t="s">
-        <v>5</v>
-      </c>
-      <c r="O22" s="7">
-        <v>3</v>
-      </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="4"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -1824,30 +1664,6 @@
       <c r="M23" s="4"/>
       <c r="N23" s="5"/>
       <c r="O23" s="4"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="4"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2 New cards. ()
</commit_message>
<xml_diff>
--- a/Assets/Excel/bibiCards.xlsx
+++ b/Assets/Excel/bibiCards.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="105">
   <si>
     <t>בטחון</t>
   </si>
@@ -207,9 +207,6 @@
     <t>חכה עם זה לאוגוסט</t>
   </si>
   <si>
-    <t>הסרט הישראלי ״הכיבוש הוא רע״ זכה בפרס הסרט הטוב ביותר (לא צפיתי)</t>
-  </si>
-  <si>
     <t>תנשמי עמוק </t>
   </si>
   <si>
@@ -225,9 +222,6 @@
     <t>תחזיר לסגול חציל</t>
   </si>
   <si>
-    <t>(נגלה אליך בחלום): ״בנימין, זוהי לא דרכי. אין מקום להסתה ולפילוג בקרב אזרחי ישראל״</t>
-  </si>
-  <si>
     <t>סבבה, אני מבטל את חוק הלאום</t>
   </si>
   <si>
@@ -288,12 +282,6 @@
     <t>נפתחה נגדך חקירה על שחיתות, אני צריך שתגיע לכאן</t>
   </si>
   <si>
-    <t>"אתה תותח"</t>
-  </si>
-  <si>
-    <t>"I Will Survive"</t>
-  </si>
-  <si>
     <t>יניב מלכה, מעצב שיער</t>
   </si>
   <si>
@@ -322,6 +310,39 @@
   </si>
   <si>
     <t>אריה דרעי</t>
+  </si>
+  <si>
+    <t>שוב יש הפגנת ענק של השמאל. הפעם: המחירים הגבוהים של שיעורי ביקראם יוגה</t>
+  </si>
+  <si>
+    <t>תשתמש בכל זרנוקי המים האפשריים</t>
+  </si>
+  <si>
+    <t>תן הוראה לכוחותינו לחלק למפגינים קוטג׳ קר</t>
+  </si>
+  <si>
+    <t>ביטן</t>
+  </si>
+  <si>
+    <t>שמפניה?</t>
+  </si>
+  <si>
+    <t>ארבעים אריזות, תודה</t>
+  </si>
+  <si>
+    <t>מאה וארבעים אריזות, תודה</t>
+  </si>
+  <si>
+    <t>נגלה בחלום: בנימין, זוהי לא דרכי. אין מקום להסתה ולפילוג בקרב אזרחי ישראל</t>
+  </si>
+  <si>
+    <t>הסרט הישראלי ״הכיבוש הוא רע״ זכה בפרס הסרט הטוב ביותר )לא צפיתי(</t>
+  </si>
+  <si>
+    <t>אתה תותח</t>
+  </si>
+  <si>
+    <t>evivruS lliW I</t>
   </si>
 </sst>
 </file>
@@ -424,7 +445,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -442,6 +463,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -723,14 +747,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="194" zoomScaleNormal="194" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="3" max="3" width="50.1640625" customWidth="1"/>
+    <col min="3" max="3" width="73.33203125" customWidth="1"/>
     <col min="4" max="4" width="31.83203125" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
@@ -793,16 +817,16 @@
         <v>31</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>73</v>
       </c>
       <c r="F2" s="7">
         <v>0</v>
@@ -843,10 +867,10 @@
         <v>45</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -884,13 +908,13 @@
         <v>34</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>78</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -928,7 +952,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>6</v>
@@ -972,7 +996,7 @@
         <v>36</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>46</v>
@@ -1060,7 +1084,7 @@
         <v>37</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>6</v>
@@ -1110,7 +1134,7 @@
         <v>50</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F9">
         <v>2</v>
@@ -1145,16 +1169,16 @@
         <v>58</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>51</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F10">
         <v>5</v>
@@ -1236,7 +1260,7 @@
         <v>38</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>55</v>
@@ -1324,13 +1348,13 @@
         <v>44</v>
       </c>
       <c r="C14" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="E14" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="F14">
         <v>5</v>
@@ -1368,13 +1392,13 @@
         <v>36</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>87</v>
+        <v>61</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>104</v>
       </c>
       <c r="F15">
         <v>5</v>
@@ -1409,16 +1433,16 @@
         <v>65</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="F16">
         <v>5</v>
@@ -1459,10 +1483,10 @@
         <v>42</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F17">
         <v>5</v>
@@ -1499,14 +1523,14 @@
       <c r="B18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>65</v>
+      <c r="C18" s="11" t="s">
+        <v>101</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F18">
         <v>10</v>
@@ -1541,16 +1565,16 @@
         <v>68</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F19">
         <v>2</v>
@@ -1585,73 +1609,134 @@
         <v>71</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C20" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="9">
+        <v>5</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20">
+        <v>5</v>
+      </c>
+      <c r="I20">
+        <v>5</v>
+      </c>
+      <c r="J20">
+        <v>5</v>
+      </c>
+      <c r="K20">
+        <v>2</v>
+      </c>
+      <c r="L20">
+        <v>5</v>
+      </c>
+      <c r="M20">
+        <v>5</v>
+      </c>
+      <c r="O20" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>80</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D21" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E21" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F20" s="9">
-        <v>5</v>
-      </c>
-      <c r="G20">
+      <c r="F21" s="4">
+        <v>2</v>
+      </c>
+      <c r="G21" s="4">
+        <v>2</v>
+      </c>
+      <c r="H21" s="4">
+        <v>10</v>
+      </c>
+      <c r="I21" s="4">
+        <v>10</v>
+      </c>
+      <c r="J21" s="4">
+        <v>5</v>
+      </c>
+      <c r="K21" s="4">
+        <v>5</v>
+      </c>
+      <c r="L21" s="4">
         <v>0</v>
       </c>
-      <c r="H20">
-        <v>5</v>
-      </c>
-      <c r="I20">
-        <v>5</v>
-      </c>
-      <c r="J20">
-        <v>5</v>
-      </c>
-      <c r="K20">
+      <c r="M21" s="4">
         <v>0</v>
       </c>
-      <c r="L20">
-        <v>5</v>
-      </c>
-      <c r="M20">
-        <v>5</v>
-      </c>
-      <c r="O20" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
       <c r="N21" s="5"/>
-      <c r="O21" s="4"/>
+      <c r="O21" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
+      <c r="A22">
+        <v>81</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" s="4">
+        <v>5</v>
+      </c>
+      <c r="G22" s="4">
+        <v>2</v>
+      </c>
+      <c r="H22" s="4">
+        <v>5</v>
+      </c>
+      <c r="I22" s="4">
+        <v>8</v>
+      </c>
+      <c r="J22" s="4">
+        <v>5</v>
+      </c>
+      <c r="K22" s="4">
+        <v>2</v>
+      </c>
+      <c r="L22" s="4">
+        <v>5</v>
+      </c>
+      <c r="M22" s="4">
+        <v>10</v>
+      </c>
       <c r="N22" s="5"/>
-      <c r="O22" s="4"/>
+      <c r="O22" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F23" s="4"/>

</xml_diff>

<commit_message>
text editing. end texts. new images
</commit_message>
<xml_diff>
--- a/Assets/Excel/bibiCards.xlsx
+++ b/Assets/Excel/bibiCards.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="108">
   <si>
     <t>בטחון</t>
   </si>
@@ -132,18 +132,9 @@
     <t>credit</t>
   </si>
   <si>
-    <t>טראמפ</t>
-  </si>
-  <si>
     <t>איילת שקד</t>
   </si>
   <si>
-    <t>יאיר נתניהו</t>
-  </si>
-  <si>
-    <t>שרה נתניהו</t>
-  </si>
-  <si>
     <t>מפכ"ל המשטרה</t>
   </si>
   <si>
@@ -270,9 +261,6 @@
     <t>תדאג שיוקם בניין על שמי בפקולטה לפסיכולוגיה באוניברסיטת תל אביב</t>
   </si>
   <si>
-    <t>נתחיל מתכנית בערוץ עשרים</t>
-  </si>
-  <si>
     <t>סורי, הכביסה של שרה לא תספיק להתייבש</t>
   </si>
   <si>
@@ -321,9 +309,6 @@
     <t>תן הוראה לכוחותינו לחלק למפגינים קוטג׳ קר</t>
   </si>
   <si>
-    <t>ביטן</t>
-  </si>
-  <si>
     <t>שמפניה?</t>
   </si>
   <si>
@@ -343,13 +328,37 @@
   </si>
   <si>
     <t>evivruS lliW I</t>
+  </si>
+  <si>
+    <t>נתחיל מתוכנית בערוץ עשרים</t>
+  </si>
+  <si>
+    <t>יש שריפות ענק בצפון. בתחקיר ראשון עולה שזאת הצתה או מנגל</t>
+  </si>
+  <si>
+    <t>הצתה</t>
+  </si>
+  <si>
+    <t>מנגל</t>
+  </si>
+  <si>
+    <t>דוד ביטן</t>
+  </si>
+  <si>
+    <t xml:space="preserve">שרה </t>
+  </si>
+  <si>
+    <t xml:space="preserve">יאיר </t>
+  </si>
+  <si>
+    <t>דונלד טראמפ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -422,6 +431,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -440,12 +455,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -466,10 +483,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -747,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="194" zoomScaleNormal="194" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="194" zoomScaleNormal="194" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -817,16 +837,16 @@
         <v>31</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>71</v>
       </c>
       <c r="F2" s="7">
         <v>0</v>
@@ -861,16 +881,16 @@
         <v>51</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -905,16 +925,16 @@
         <v>52</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -952,7 +972,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>6</v>
@@ -993,16 +1013,16 @@
         <v>54</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -1037,10 +1057,10 @@
         <v>55</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>6</v>
@@ -1081,10 +1101,10 @@
         <v>56</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>37</v>
+        <v>105</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>6</v>
@@ -1125,16 +1145,16 @@
         <v>57</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="F9">
         <v>2</v>
@@ -1169,16 +1189,16 @@
         <v>58</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F10">
         <v>5</v>
@@ -1216,13 +1236,13 @@
         <v>13</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1257,16 +1277,16 @@
         <v>61</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F12">
         <v>5</v>
@@ -1301,16 +1321,16 @@
         <v>62</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -1345,16 +1365,16 @@
         <v>63</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F14">
         <v>5</v>
@@ -1389,16 +1409,16 @@
         <v>64</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F15">
         <v>5</v>
@@ -1433,16 +1453,16 @@
         <v>65</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F16">
         <v>5</v>
@@ -1480,13 +1500,13 @@
         <v>13</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F17">
         <v>5</v>
@@ -1521,16 +1541,16 @@
         <v>67</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F18">
         <v>10</v>
@@ -1565,16 +1585,16 @@
         <v>68</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F19">
         <v>2</v>
@@ -1609,16 +1629,16 @@
         <v>71</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F20" s="9">
         <v>5</v>
@@ -1653,16 +1673,16 @@
         <v>80</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F21" s="4">
         <v>2</v>
@@ -1698,16 +1718,16 @@
         <v>81</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F22" s="4">
         <v>5</v>
@@ -1738,15 +1758,46 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
+    <row r="23" spans="1:15" ht="19" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>83</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F23" s="4">
+        <v>2</v>
+      </c>
+      <c r="G23" s="4">
+        <v>2</v>
+      </c>
+      <c r="H23" s="4">
+        <v>8</v>
+      </c>
+      <c r="I23" s="4">
+        <v>5</v>
+      </c>
+      <c r="J23" s="4">
+        <v>2</v>
+      </c>
+      <c r="K23" s="4">
+        <v>2</v>
+      </c>
+      <c r="L23" s="4">
+        <v>2</v>
+      </c>
+      <c r="M23" s="4">
+        <v>5</v>
+      </c>
       <c r="N23" s="5"/>
       <c r="O23" s="4"/>
     </row>

</xml_diff>